<commit_message>
CIERRE  DEL  23 nOV-21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/CREDITOS  4 CARNES HERRADURA  NOVIEMBRE     2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 11  NOVIEMBRE 2021/CREDITOS  4 CARNES HERRADURA  NOVIEMBRE     2021.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES  AGOSTO   2021    " sheetId="1" r:id="rId1"/>
     <sheet name="REMISIONES  SEPTIEMBRE  2021  " sheetId="2" r:id="rId2"/>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja2" sheetId="3" r:id="rId4"/>
+    <sheet name="REMISIONES NOVIEMBRE   2021   " sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <r>
       <t xml:space="preserve">REMISIONES    POR     CREDITOS         DE   </t>
@@ -262,6 +263,36 @@
   </si>
   <si>
     <t>HERRADURA DAVID</t>
+  </si>
+  <si>
+    <r>
+      <t>REMISIONES    POR     CREDITOS         DE    NOVIEMBRE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        2 0 2 1</t>
+    </r>
+  </si>
+  <si>
+    <t>DAVID HERRADURA</t>
   </si>
 </sst>
 </file>
@@ -655,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -825,6 +856,10 @@
     <xf numFmtId="166" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1182,6 +1217,117 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>647703</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="1 Conector recto de flecha">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4576765" y="6748465"/>
+          <a:ext cx="581022" cy="590546"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561977</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>123829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>161927</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="2 Conector recto de flecha">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5472114" y="6796092"/>
+          <a:ext cx="638173" cy="495298"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -3553,8 +3699,8 @@
   </sheetPr>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4208,11 +4354,15 @@
       <c r="E26" s="21">
         <v>7970</v>
       </c>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="F26" s="63">
+        <v>44508</v>
+      </c>
+      <c r="G26" s="64">
+        <v>7970</v>
+      </c>
       <c r="H26" s="19">
         <f t="shared" si="0"/>
-        <v>7970</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4515,11 +4665,11 @@
       <c r="F49" s="41"/>
       <c r="G49" s="41">
         <f>SUM(G4:G48)</f>
-        <v>148502</v>
+        <v>156472</v>
       </c>
       <c r="H49" s="42">
         <f>SUM(H4:H48)</f>
-        <v>7970</v>
+        <v>0</v>
       </c>
       <c r="I49" s="2"/>
     </row>
@@ -4563,7 +4713,7 @@
       <c r="D53" s="2"/>
       <c r="E53" s="69">
         <f>E49-G49</f>
-        <v>7970</v>
+        <v>0</v>
       </c>
       <c r="F53" s="70"/>
       <c r="G53" s="71"/>
@@ -4703,6 +4853,951 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="13.140625" style="54" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="55" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="57" customWidth="1"/>
+    <col min="7" max="7" width="18" style="58" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="67"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="B2" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="46.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>44508</v>
+      </c>
+      <c r="B4" s="13">
+        <v>61</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="16">
+        <v>5798</v>
+      </c>
+      <c r="F4" s="17">
+        <v>44509</v>
+      </c>
+      <c r="G4" s="18">
+        <v>5798</v>
+      </c>
+      <c r="H4" s="19">
+        <f t="shared" ref="H4:H48" si="0">E4-G4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>44509</v>
+      </c>
+      <c r="B5" s="13">
+        <f>B4+1</f>
+        <v>62</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="21">
+        <v>7963</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="19">
+        <f t="shared" si="0"/>
+        <v>7963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13">
+        <f t="shared" ref="B6:B26" si="1">B5+1</f>
+        <v>63</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="13">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="36">
+        <v>0</v>
+      </c>
+      <c r="F48" s="37"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="39"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="41">
+        <f>SUM(E4:E48)</f>
+        <v>13761</v>
+      </c>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41">
+        <f>SUM(G4:G48)</f>
+        <v>5798</v>
+      </c>
+      <c r="H49" s="42">
+        <f>SUM(H4:H48)</f>
+        <v>7963</v>
+      </c>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="39"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="39"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="44"/>
+      <c r="G51" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="46"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="39"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="69">
+        <f>E49-G49</f>
+        <v>7963</v>
+      </c>
+      <c r="F53" s="70"/>
+      <c r="G53" s="71"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B55" s="39"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="39"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="31"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="52"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="39"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="45"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="39"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="45"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="39"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="45"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="39"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="45"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="39"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="45"/>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="39"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="45"/>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="39"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="45"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="39"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="45"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="39"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="45"/>
+      <c r="I66" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E55:G55"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>